<commit_message>
Completed EndScreen() Score Tracking
</commit_message>
<xml_diff>
--- a/assets/8085 ISA.xlsx
+++ b/assets/8085 ISA.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28025"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28129"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="H:\My Drive\Programming\Java\IdeaProjects\8085 ISA Test\assets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2A7043D1-19C1-4FA1-8E72-9F9638E8AC7A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DF4DCFCF-A7E2-4F45-AB3A-C9BB9A9B34C4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{3B1F1732-86DF-4257-B8CB-601647F5C8B3}"/>
   </bookViews>
@@ -187,6 +187,232 @@
     <t>Rotate the accumulator right through carry</t>
   </si>
   <si>
+    <t>Rotate the accumulator left through carry</t>
+  </si>
+  <si>
+    <t>Rotate the accumulator right</t>
+  </si>
+  <si>
+    <t>Rotate the accumulator left</t>
+  </si>
+  <si>
+    <r>
+      <t>Each binary bit of the accumulator is rotated left by one position. Bit D</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="subscript"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>7</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> is placed in the position of D</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="subscript"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>0</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> as well as in the Carry flag. CY is modified according to bit D</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="subscript"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>7</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>Each binary bit of the accumulator is rotated right by one position. Bit D</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="subscript"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>0</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> is placed in the position of D</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="subscript"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>7</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> as well as in the Carry flag. CY is modified according to bit D</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="subscript"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>0</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>.</t>
+    </r>
+  </si>
+  <si>
+    <t>Logical OR immediate with the accumulator</t>
+  </si>
+  <si>
+    <t>Logical OR register or Memory with the accumulator</t>
+  </si>
+  <si>
+    <t>Exclusive OR immediate with the accumulator</t>
+  </si>
+  <si>
+    <t>Exclusive OR register or Memory with the accumulator</t>
+  </si>
+  <si>
+    <t>Logical AND immediate with the accumulator</t>
+  </si>
+  <si>
+    <t>The contents of the accumulator are logically OR with the 8-bit data and the result is placed in the accumulator.</t>
+  </si>
+  <si>
+    <t>The contents of the accumulator are logically OR with M the contents of the register or memory, and result is placed in the accumulator.</t>
+  </si>
+  <si>
+    <t>The contents of the accumulator are Exclusive OR with the 8-bit data and the result is placed in the accumulator.</t>
+  </si>
+  <si>
+    <t>The contents of the accumulator are Exclusive OR with M the contents of the register or memory, and the result is placed in the accumulator.</t>
+  </si>
+  <si>
+    <t>The contents of the accumulator are logically AND with the 8-bit data and the result is placed in the accumulator.</t>
+  </si>
+  <si>
+    <t>FUNCTION</t>
+  </si>
+  <si>
+    <r>
+      <t>Each binary bit of the accumulator is rotated left by one position through the Carry flag. Bit D</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="subscript"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>7</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> is placed in the Carry flag, and the Carry flag is placed in the least significant position D</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="subscript"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>0.</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> CY is modified according to bit D</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="subscript"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>7</t>
+    </r>
+  </si>
+  <si>
     <r>
       <t>Each binary bit of the accumulator is rotated right by one position through the Carry flag. Bit D</t>
     </r>
@@ -220,7 +446,7 @@
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t>7</t>
+      <t>7.</t>
     </r>
     <r>
       <rPr>
@@ -253,232 +479,6 @@
       </rPr>
       <t>.</t>
     </r>
-  </si>
-  <si>
-    <t>Rotate the accumulator left through carry</t>
-  </si>
-  <si>
-    <t>Rotate the accumulator right</t>
-  </si>
-  <si>
-    <t>Rotate the accumulator left</t>
-  </si>
-  <si>
-    <r>
-      <t>Each binary bit of the accumulator is rotated left by one position. Bit D</t>
-    </r>
-    <r>
-      <rPr>
-        <vertAlign val="subscript"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>7</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> is placed in the position of D</t>
-    </r>
-    <r>
-      <rPr>
-        <vertAlign val="subscript"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>0</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> as well as in the Carry flag. CY is modified according to bit D</t>
-    </r>
-    <r>
-      <rPr>
-        <vertAlign val="subscript"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>7</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t>Each binary bit of the accumulator is rotated right by one position. Bit D</t>
-    </r>
-    <r>
-      <rPr>
-        <vertAlign val="subscript"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>0</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> is placed in the position of D</t>
-    </r>
-    <r>
-      <rPr>
-        <vertAlign val="subscript"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>7</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> as well as in the Carry flag. CY is modified according to bit D</t>
-    </r>
-    <r>
-      <rPr>
-        <vertAlign val="subscript"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>0</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>.</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t>Each binary bit of the accumulator is rotated left by one position through the Carry flag. Bit D</t>
-    </r>
-    <r>
-      <rPr>
-        <vertAlign val="subscript"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>7</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> is placed in the Carry flag, and the Carry flag is placed in the least significant position D</t>
-    </r>
-    <r>
-      <rPr>
-        <vertAlign val="subscript"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>0</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> CY is modified according to bit D</t>
-    </r>
-    <r>
-      <rPr>
-        <vertAlign val="subscript"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>7</t>
-    </r>
-  </si>
-  <si>
-    <t>Logical OR immediate with the accumulator</t>
-  </si>
-  <si>
-    <t>Logical OR register or Memory with the accumulator</t>
-  </si>
-  <si>
-    <t>Exclusive OR immediate with the accumulator</t>
-  </si>
-  <si>
-    <t>Exclusive OR register or Memory with the accumulator</t>
-  </si>
-  <si>
-    <t>Logical AND immediate with the accumulator</t>
-  </si>
-  <si>
-    <t>The contents of the accumulator are logically OR with the 8-bit data and the result is placed in the accumulator.</t>
-  </si>
-  <si>
-    <t>The contents of the accumulator are logically OR with M the contents of the register or memory, and result is placed in the accumulator.</t>
-  </si>
-  <si>
-    <t>The contents of the accumulator are Exclusive OR with the 8-bit data and the result is placed in the accumulator.</t>
-  </si>
-  <si>
-    <t>The contents of the accumulator are Exclusive OR with M the contents of the register or memory, and the result is placed in the accumulator.</t>
-  </si>
-  <si>
-    <t>The contents of the accumulator are logically AND with the 8-bit data and the result is placed in the accumulator.</t>
-  </si>
-  <si>
-    <t>FUNCTION</t>
   </si>
 </sst>
 </file>
@@ -1345,8 +1345,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{94632ECF-11B0-4FCD-A009-75BBFC17C4DF}">
   <dimension ref="A1:E24"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D1" sqref="D1"/>
+    <sheetView tabSelected="1" topLeftCell="A17" workbookViewId="0">
+      <selection activeCell="D24" sqref="D24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1370,7 +1370,7 @@
         <v>2</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="E1" s="1" t="s">
         <v>3</v>
@@ -1540,10 +1540,10 @@
         <v>27</v>
       </c>
       <c r="D13" s="2" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="E13" s="2" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
     </row>
     <row r="14" spans="1:5" ht="57.6" x14ac:dyDescent="0.3">
@@ -1557,10 +1557,10 @@
         <v>25</v>
       </c>
       <c r="D14" s="2" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="E14" s="2" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
     </row>
     <row r="15" spans="1:5" ht="43.2" x14ac:dyDescent="0.3">
@@ -1574,10 +1574,10 @@
         <v>27</v>
       </c>
       <c r="D15" s="2" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="E15" s="2" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
     </row>
     <row r="16" spans="1:5" ht="57.6" x14ac:dyDescent="0.3">
@@ -1591,10 +1591,10 @@
         <v>25</v>
       </c>
       <c r="D16" s="2" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="E16" s="2" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
     </row>
     <row r="17" spans="1:5" ht="43.2" x14ac:dyDescent="0.3">
@@ -1608,10 +1608,10 @@
         <v>27</v>
       </c>
       <c r="D17" s="2" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="E17" s="2" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
     </row>
     <row r="18" spans="1:5" ht="61.2" x14ac:dyDescent="0.3">
@@ -1625,10 +1625,10 @@
         <v>41</v>
       </c>
       <c r="D18" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="E18" s="2" t="s">
         <v>58</v>
-      </c>
-      <c r="E18" s="2" t="s">
-        <v>59</v>
       </c>
     </row>
     <row r="19" spans="1:5" ht="61.2" x14ac:dyDescent="0.3">
@@ -1642,10 +1642,10 @@
         <v>41</v>
       </c>
       <c r="D19" s="2" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="E19" s="2" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
     <row r="20" spans="1:5" ht="75.599999999999994" x14ac:dyDescent="0.3">
@@ -1659,10 +1659,10 @@
         <v>41</v>
       </c>
       <c r="D20" s="2" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="E20" s="2" t="s">
-        <v>61</v>
+        <v>71</v>
       </c>
     </row>
     <row r="21" spans="1:5" ht="75.599999999999994" x14ac:dyDescent="0.3">
@@ -1679,7 +1679,7 @@
         <v>54</v>
       </c>
       <c r="E21" s="2" t="s">
-        <v>55</v>
+        <v>72</v>
       </c>
     </row>
     <row r="22" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
Updated the .csv & .xlsx files with the rest of the instructions.
</commit_message>
<xml_diff>
--- a/assets/8085 ISA.xlsx
+++ b/assets/8085 ISA.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="H:\My Drive\Programming\Java\IdeaProjects\8085 ISA Test\assets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DF4DCFCF-A7E2-4F45-AB3A-C9BB9A9B34C4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{28EC4806-D2A5-49CD-BC55-B6C54294E67D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{3B1F1732-86DF-4257-B8CB-601647F5C8B3}"/>
+    <workbookView xWindow="11520" yWindow="0" windowWidth="11520" windowHeight="12360" xr2:uid="{3B1F1732-86DF-4257-B8CB-601647F5C8B3}"/>
   </bookViews>
   <sheets>
     <sheet name="M&amp;M ISA" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="110" uniqueCount="73">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="405" uniqueCount="262">
   <si>
     <t>TYPE</t>
   </si>
@@ -97,9 +97,6 @@
     <t>CMP</t>
   </si>
   <si>
-    <t>R M</t>
-  </si>
-  <si>
     <t>CPI</t>
   </si>
   <si>
@@ -148,22 +145,10 @@
     <t>None</t>
   </si>
   <si>
-    <t>Compare the register or Memory with the accumulator</t>
-  </si>
-  <si>
     <t>Compare immediate with the accumulator</t>
   </si>
   <si>
-    <t>The contents of the operand (register or memory) are M compared with the contents of the accumulator.</t>
-  </si>
-  <si>
     <t>The second byte data is compared with the contents of the accumulator.</t>
-  </si>
-  <si>
-    <t>Logical AND register or Memory with the accumulator</t>
-  </si>
-  <si>
-    <t>The contents of the accumulator are logically AND with M the contents of the register or memory, and the result is placed in the accumulator.</t>
   </si>
   <si>
     <t>Set Carry</t>
@@ -325,9 +310,6 @@
     <t>Logical OR immediate with the accumulator</t>
   </si>
   <si>
-    <t>Logical OR register or Memory with the accumulator</t>
-  </si>
-  <si>
     <t>Exclusive OR immediate with the accumulator</t>
   </si>
   <si>
@@ -340,13 +322,7 @@
     <t>The contents of the accumulator are logically OR with the 8-bit data and the result is placed in the accumulator.</t>
   </si>
   <si>
-    <t>The contents of the accumulator are logically OR with M the contents of the register or memory, and result is placed in the accumulator.</t>
-  </si>
-  <si>
     <t>The contents of the accumulator are Exclusive OR with the 8-bit data and the result is placed in the accumulator.</t>
-  </si>
-  <si>
-    <t>The contents of the accumulator are Exclusive OR with M the contents of the register or memory, and the result is placed in the accumulator.</t>
   </si>
   <si>
     <t>The contents of the accumulator are logically AND with the 8-bit data and the result is placed in the accumulator.</t>
@@ -479,6 +455,605 @@
       </rPr>
       <t>.</t>
     </r>
+  </si>
+  <si>
+    <t>BI</t>
+  </si>
+  <si>
+    <t>JMP</t>
+  </si>
+  <si>
+    <t>JC</t>
+  </si>
+  <si>
+    <t>JNC</t>
+  </si>
+  <si>
+    <t>JP</t>
+  </si>
+  <si>
+    <t>JM</t>
+  </si>
+  <si>
+    <t>JZ</t>
+  </si>
+  <si>
+    <t>JNZ</t>
+  </si>
+  <si>
+    <t>JPE</t>
+  </si>
+  <si>
+    <t>JPO</t>
+  </si>
+  <si>
+    <t>CALL</t>
+  </si>
+  <si>
+    <t>CC</t>
+  </si>
+  <si>
+    <t>CNC</t>
+  </si>
+  <si>
+    <t>CP</t>
+  </si>
+  <si>
+    <t>CM</t>
+  </si>
+  <si>
+    <t>CZ</t>
+  </si>
+  <si>
+    <t>CNZ</t>
+  </si>
+  <si>
+    <t>CPE</t>
+  </si>
+  <si>
+    <t>CPO</t>
+  </si>
+  <si>
+    <t>RET</t>
+  </si>
+  <si>
+    <t>RC</t>
+  </si>
+  <si>
+    <t>RNC</t>
+  </si>
+  <si>
+    <t>RP</t>
+  </si>
+  <si>
+    <t>RM</t>
+  </si>
+  <si>
+    <t>RZ</t>
+  </si>
+  <si>
+    <t>RNZ</t>
+  </si>
+  <si>
+    <t>RPE</t>
+  </si>
+  <si>
+    <t>RPO</t>
+  </si>
+  <si>
+    <t>PCHL</t>
+  </si>
+  <si>
+    <t>RST</t>
+  </si>
+  <si>
+    <t>16-bit address</t>
+  </si>
+  <si>
+    <t>0-7</t>
+  </si>
+  <si>
+    <t>Jump unconditinally</t>
+  </si>
+  <si>
+    <t>Jump on carry</t>
+  </si>
+  <si>
+    <t>Jump on no carry</t>
+  </si>
+  <si>
+    <t>Jump on positive</t>
+  </si>
+  <si>
+    <t>Jump on minus</t>
+  </si>
+  <si>
+    <t>Jump on zero</t>
+  </si>
+  <si>
+    <t>Jump on no zero</t>
+  </si>
+  <si>
+    <t>Jump on parity even</t>
+  </si>
+  <si>
+    <t>Jump on parity odd</t>
+  </si>
+  <si>
+    <t>Call subroutine unconditionally</t>
+  </si>
+  <si>
+    <t>Call on carry</t>
+  </si>
+  <si>
+    <t>Call on no carry</t>
+  </si>
+  <si>
+    <t>Call on positive</t>
+  </si>
+  <si>
+    <t>Call on minus</t>
+  </si>
+  <si>
+    <t>Call on zero</t>
+  </si>
+  <si>
+    <t>Call on no zero</t>
+  </si>
+  <si>
+    <t>Call on parity even</t>
+  </si>
+  <si>
+    <t>Call on parity odd</t>
+  </si>
+  <si>
+    <t>Return from subroutine unconditionally</t>
+  </si>
+  <si>
+    <t>Return on carry</t>
+  </si>
+  <si>
+    <t>Return on no carry</t>
+  </si>
+  <si>
+    <t>Return on positive</t>
+  </si>
+  <si>
+    <t>Return on minus</t>
+  </si>
+  <si>
+    <t>Return on zero</t>
+  </si>
+  <si>
+    <t>Return on no zero</t>
+  </si>
+  <si>
+    <t>Return on parity even</t>
+  </si>
+  <si>
+    <t>Return on parity odd</t>
+  </si>
+  <si>
+    <t>Load the program counter with HL contents</t>
+  </si>
+  <si>
+    <t>Restart</t>
+  </si>
+  <si>
+    <t>The program sequence is transferred to the memory address given in the operand.</t>
+  </si>
+  <si>
+    <t>The program sequence is transferred to the memory address given in the operand if CY=1.</t>
+  </si>
+  <si>
+    <t>The program sequence is transferred to the memory address given in the operand if CY=0.</t>
+  </si>
+  <si>
+    <t>The program sequence is transferred to the memory address given in the operand if S=0.</t>
+  </si>
+  <si>
+    <t>The program sequence is transferred to the memory address given in the operand if S=1.</t>
+  </si>
+  <si>
+    <t>The program sequence is transferred to the memory address given in the operand if Z=0.</t>
+  </si>
+  <si>
+    <t>The program sequence is transferred to the memory address given in the operand if Z=1.</t>
+  </si>
+  <si>
+    <t>The program sequence is transferred to the memory address given in the operand if P=1.</t>
+  </si>
+  <si>
+    <t>The program sequence is transferred to the memory address given in the operand if P=0.</t>
+  </si>
+  <si>
+    <t>The contents of registers H &amp; L are copied into the program counter. The contents of H are placed as the high-order byte and the contents of L as the low order byte.</t>
+  </si>
+  <si>
+    <t>The program control is transferred to the subroutine present in the given memory address.</t>
+  </si>
+  <si>
+    <t>The program control is transferred to the subroutine present in the given memory address if CY=1.</t>
+  </si>
+  <si>
+    <t>The program control is transferred to the subroutine present in the given memory address if CY=0.</t>
+  </si>
+  <si>
+    <t>The program control is transferred to the subroutine present in the given memory address if S=0.</t>
+  </si>
+  <si>
+    <t>The program control is transferred to the subroutine present in the given memory address if S=1.</t>
+  </si>
+  <si>
+    <t>The program control is transferred to the subroutine present in the given memory address if Z=1.</t>
+  </si>
+  <si>
+    <t>The program control is transferred to the subroutine present in the given memory address if Z=0.</t>
+  </si>
+  <si>
+    <t>The program control is transferred to the subroutine present in the given memory address if P=1.</t>
+  </si>
+  <si>
+    <t>The program control is transferred to the subroutine present in the given memory address if P=0.</t>
+  </si>
+  <si>
+    <t>The program control is returned from the subroutine to the calling program.</t>
+  </si>
+  <si>
+    <t>The program control is returned from the subroutine to the calling program if CY=1.</t>
+  </si>
+  <si>
+    <t>The program control is returned from the subroutine to the calling program if CY=0.</t>
+  </si>
+  <si>
+    <t>The program control is returned from the subroutine to the calling program if S=0.</t>
+  </si>
+  <si>
+    <t>The program control is returned from the subroutine to the calling program if S=1.</t>
+  </si>
+  <si>
+    <t>The program control is returned from the subroutine to the calling program if Z=1.</t>
+  </si>
+  <si>
+    <t>The program control is returned from the subroutine to the calling program if Z=0.</t>
+  </si>
+  <si>
+    <t>The program control is returned from the subroutine to the calling program if P=1.</t>
+  </si>
+  <si>
+    <t>The program control is returned from the subroutine to the calling program if P=0.</t>
+  </si>
+  <si>
+    <t>The RST instruction is used as software instructions in a program to transfer the program execution to one of the following eight locations based on the operand: 0000H, 0008H, 0010H, 0018H, 0020H, 0028H, 0030H &amp; 0038H.</t>
+  </si>
+  <si>
+    <t>AI</t>
+  </si>
+  <si>
+    <t>ADD</t>
+  </si>
+  <si>
+    <t>ADC</t>
+  </si>
+  <si>
+    <t>ADI</t>
+  </si>
+  <si>
+    <t>ACI</t>
+  </si>
+  <si>
+    <t>DAD</t>
+  </si>
+  <si>
+    <t>SUB</t>
+  </si>
+  <si>
+    <t>SBB</t>
+  </si>
+  <si>
+    <t>SUI</t>
+  </si>
+  <si>
+    <t>SBI</t>
+  </si>
+  <si>
+    <t>INX</t>
+  </si>
+  <si>
+    <t>DCR</t>
+  </si>
+  <si>
+    <t>DCX</t>
+  </si>
+  <si>
+    <t>DAA</t>
+  </si>
+  <si>
+    <t>INR</t>
+  </si>
+  <si>
+    <t>MOV</t>
+  </si>
+  <si>
+    <t>MVI</t>
+  </si>
+  <si>
+    <t>LDA</t>
+  </si>
+  <si>
+    <t>LDAX</t>
+  </si>
+  <si>
+    <t>LXI</t>
+  </si>
+  <si>
+    <t>LHLD</t>
+  </si>
+  <si>
+    <t>STA</t>
+  </si>
+  <si>
+    <t>STAX</t>
+  </si>
+  <si>
+    <t>SHLD</t>
+  </si>
+  <si>
+    <t>XCHG</t>
+  </si>
+  <si>
+    <t>SPHL</t>
+  </si>
+  <si>
+    <t>XTHL</t>
+  </si>
+  <si>
+    <t>PUSH</t>
+  </si>
+  <si>
+    <t>POP</t>
+  </si>
+  <si>
+    <t>OUT</t>
+  </si>
+  <si>
+    <t>IN</t>
+  </si>
+  <si>
+    <t>DTI</t>
+  </si>
+  <si>
+    <t>Reg. pair</t>
+  </si>
+  <si>
+    <t>R</t>
+  </si>
+  <si>
+    <t>B/D Reg. pair</t>
+  </si>
+  <si>
+    <t>Reg. pair, 16-bit data</t>
+  </si>
+  <si>
+    <t>8-bit port address</t>
+  </si>
+  <si>
+    <t>Dt, Sc</t>
+  </si>
+  <si>
+    <t>Copy to Destination (Dt) from Source (Sc)</t>
+  </si>
+  <si>
+    <t>Dt, 8-bit data</t>
+  </si>
+  <si>
+    <t>Move immediate 8-bit data to destination (Dt)</t>
+  </si>
+  <si>
+    <t>Load the accumulator</t>
+  </si>
+  <si>
+    <t>Load the accumulator indirect</t>
+  </si>
+  <si>
+    <t>Load the register pair with immediate</t>
+  </si>
+  <si>
+    <t>Load H &amp; L registers direct</t>
+  </si>
+  <si>
+    <t>Store the accumulator</t>
+  </si>
+  <si>
+    <t>Store the accumulator indirect</t>
+  </si>
+  <si>
+    <t>Store H &amp; L registers direct</t>
+  </si>
+  <si>
+    <t>Exchange H &amp; L with D &amp; E</t>
+  </si>
+  <si>
+    <t>Copy H &amp; L registers to the stack pointer</t>
+  </si>
+  <si>
+    <t>Exchange H &amp; L with the top of stack</t>
+  </si>
+  <si>
+    <t>Push register pair onto the stack</t>
+  </si>
+  <si>
+    <t>Pop off stack to the register pair</t>
+  </si>
+  <si>
+    <t>Output the data from the accumulator to a port with 8-bit address</t>
+  </si>
+  <si>
+    <t>Input the data from the accumulator to a port with 8-bit address</t>
+  </si>
+  <si>
+    <t>The contents of the operand (register or memory) are compared with the contents of the accumulator.</t>
+  </si>
+  <si>
+    <t>Compare the register or memory with the accumulator</t>
+  </si>
+  <si>
+    <t>Logical AND register or memory with the accumulator</t>
+  </si>
+  <si>
+    <t>The contents of the accumulator are logically AND with the contents of the register or memory, and the result is placed in the accumulator.</t>
+  </si>
+  <si>
+    <t>The contents of the accumulator are Exclusive OR with the contents of the register or memory, and the result is placed in the accumulator.</t>
+  </si>
+  <si>
+    <t>Logical OR register or memory with the accumulator</t>
+  </si>
+  <si>
+    <t>The contents of the accumulator are logically OR with the contents of the register or memory, and result is placed in the accumulator.</t>
+  </si>
+  <si>
+    <t>R/M</t>
+  </si>
+  <si>
+    <t>Add register or memory to the accumulator</t>
+  </si>
+  <si>
+    <t>Add register or memory to the accumulator with carry</t>
+  </si>
+  <si>
+    <t>Add the immediate to the accumulator</t>
+  </si>
+  <si>
+    <t>Add the immediate to the accumulator with carry</t>
+  </si>
+  <si>
+    <t>Add the register pair to HL registers</t>
+  </si>
+  <si>
+    <t>Subtract the register or memory from the accumulator</t>
+  </si>
+  <si>
+    <t>Subtract the register or memory &amp; borrow from the accumulator</t>
+  </si>
+  <si>
+    <t>Subtract the immediate from the accumulator</t>
+  </si>
+  <si>
+    <t>Subtract the immediate &amp; borrow from the accumulator</t>
+  </si>
+  <si>
+    <t>Increment the register or memory by 1</t>
+  </si>
+  <si>
+    <t>Increment register pair by 1</t>
+  </si>
+  <si>
+    <t>Decrement register pair by 1</t>
+  </si>
+  <si>
+    <t>Decrement the register or memory by 1</t>
+  </si>
+  <si>
+    <t>Decimal adjust accumulator</t>
+  </si>
+  <si>
+    <t>The contents of the register or memory are added to the contents of the accumulator and the result is stored in the accumulator.</t>
+  </si>
+  <si>
+    <t>The contents of the register or memory &amp; the carry flag are added to the contents of the accumulator and the
+result is stored in the accumulator.</t>
+  </si>
+  <si>
+    <t>The 8-bit data is added to the contents of the accumulator and the result is stored in the accumulator.</t>
+  </si>
+  <si>
+    <t>The 8-bit data &amp; the carry flag are added to the contents of the accumulator and the result is stored in the accumulator.</t>
+  </si>
+  <si>
+    <t>The 16-bit data of the specified register pair are added to the contents of the HL register.</t>
+  </si>
+  <si>
+    <t>The contents of the register or the memory are subtracted from the contents of the accumulator, and the result is stored in the accumulator.</t>
+  </si>
+  <si>
+    <t>The contents of the register or the memory &amp; the borrow flag are subtracted from the contents of the accumulator and the result is placed in the accumulator.</t>
+  </si>
+  <si>
+    <t>The 8-bit data is subtracted from the contents of the accumulator and the result is stored in the accumulator.</t>
+  </si>
+  <si>
+    <t>The contents of register H are exchanged with the contents of register D, and the contents of register L are exchanged with the contents of register E.</t>
+  </si>
+  <si>
+    <t>The 8-bit data &amp; the borrow flag are subtracted from the contents of the accumulator and the result is placed in the accumulator.</t>
+  </si>
+  <si>
+    <t>The contents of the designated register or the memory are incremented by 1.</t>
+  </si>
+  <si>
+    <t>The contents of the designated register pair are incremented by 1.</t>
+  </si>
+  <si>
+    <t>The contents of the designated register pair are decremented by 1.</t>
+  </si>
+  <si>
+    <t>The contents of the designated register or memory are decremented by 1.</t>
+  </si>
+  <si>
+    <t>The contents of the accumulator are changed from a binary value to two 4-bit BCD digits.
+If the value of the low-order 4-bits in the accumulator is greater than 9 or if AC flag is set, the instruction adds 6 to the low-order four bits.
+If the value of the high-order 4-bits in the accumulator is greater than 9 or if the Carry flag is set, the instruction adds 6 to the high-order four bits.</t>
+  </si>
+  <si>
+    <t>This instruction copies the contents of the source register or memory into the destination register or memory without any alteration.</t>
+  </si>
+  <si>
+    <t>The 8-bit data is stored in the destination register or memory.</t>
+  </si>
+  <si>
+    <t>The contents of the designated register pair point to a memory location. This instruction copies the contents of that memory location into the accumulator.</t>
+  </si>
+  <si>
+    <t>The contents of a memory location, specified by a 16-bit address in the operand, are copied to the accumulator.</t>
+  </si>
+  <si>
+    <t>The instruction loads the 16-bit data in the designated register pair.</t>
+  </si>
+  <si>
+    <t>The instruction copies the contents of the memory location pointed out by the address into register L and copies the contents of the next memory location into register H.</t>
+  </si>
+  <si>
+    <t>The contents of the accumulator are copied into the memory location specified by the operand.</t>
+  </si>
+  <si>
+    <t>The contents of the accumulator are copied into the memory location specified by the contents of the operand.</t>
+  </si>
+  <si>
+    <t>The contents of register L are stored in the memory location specified by the 16-bit address in the operand and the contents of H register are stored into the next memory location by incrementing the operand.</t>
+  </si>
+  <si>
+    <t>The instruction loads the contents of the H &amp; L registers into the stack pointer register. The contents of the H register provide the high-order address and the contents of the L register provide the low-order address.</t>
+  </si>
+  <si>
+    <t>The contents of the L register are exchanged with the stack location pointed out by the contents of the stack pointer register.
+The contents of the H register are exchanged with the next stack location (SP+1).</t>
+  </si>
+  <si>
+    <t>The contents of the register pair designated in the operand are copied onto the stack in the following sequence.
+The stack pointer register is decremented and the contents of the high order register (B, D, H. A) are copied into that location.
+The stack pointer register is decremented again and the contents of the low-order register (C, E, L, flags) are copied to that location.</t>
+  </si>
+  <si>
+    <t>The contents of the memory location pointed out by the stack pointer register are copied to the low-order register (C, E, L, status flags) of the operand.
+The stack pointer is incremented by 1 and the contents of that memory location are copied to the high-order register (B, D, H, A) of the operand.
+The stack pointer register is again incremented by 1.</t>
+  </si>
+  <si>
+    <t>The contents of the input port designated in the operand are read and loaded into the accumulator.</t>
+  </si>
+  <si>
+    <t>The contents of the accumulator are copied into the I/O port specified by the operand.</t>
   </si>
 </sst>
 </file>
@@ -1343,10 +1918,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{94632ECF-11B0-4FCD-A009-75BBFC17C4DF}">
-  <dimension ref="A1:E24"/>
+  <dimension ref="A1:E86"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A17" workbookViewId="0">
-      <selection activeCell="D24" sqref="D24"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A83" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="E86" sqref="E86"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1370,7 +1946,7 @@
         <v>2</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>70</v>
+        <v>62</v>
       </c>
       <c r="E1" s="1" t="s">
         <v>3</v>
@@ -1384,7 +1960,7 @@
         <v>5</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="D3" s="2" t="s">
         <v>6</v>
@@ -1401,7 +1977,7 @@
         <v>8</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="D4" s="2" t="s">
         <v>9</v>
@@ -1418,7 +1994,7 @@
         <v>11</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="D5" s="2" t="s">
         <v>12</v>
@@ -1435,7 +2011,7 @@
         <v>14</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="D6" s="2" t="s">
         <v>15</v>
@@ -1452,7 +2028,7 @@
         <v>17</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="D7" s="2" t="s">
         <v>18</v>
@@ -1469,7 +2045,7 @@
         <v>20</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="D8" s="2" t="s">
         <v>21</v>
@@ -1486,13 +2062,13 @@
         <v>24</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>25</v>
+        <v>217</v>
       </c>
       <c r="D10" s="2" t="s">
-        <v>42</v>
+        <v>211</v>
       </c>
       <c r="E10" s="2" t="s">
-        <v>44</v>
+        <v>210</v>
       </c>
     </row>
     <row r="11" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
@@ -1500,16 +2076,16 @@
         <v>23</v>
       </c>
       <c r="B11" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="C11" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="C11" s="2" t="s">
-        <v>27</v>
-      </c>
       <c r="D11" s="2" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="E11" s="2" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
     </row>
     <row r="12" spans="1:5" ht="57.6" x14ac:dyDescent="0.3">
@@ -1517,16 +2093,16 @@
         <v>23</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C12" s="2" t="s">
-        <v>25</v>
+        <v>217</v>
       </c>
       <c r="D12" s="2" t="s">
-        <v>46</v>
+        <v>212</v>
       </c>
       <c r="E12" s="2" t="s">
-        <v>47</v>
+        <v>213</v>
       </c>
     </row>
     <row r="13" spans="1:5" ht="43.2" x14ac:dyDescent="0.3">
@@ -1534,33 +2110,33 @@
         <v>23</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C13" s="2" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="D13" s="2" t="s">
-        <v>64</v>
+        <v>58</v>
       </c>
       <c r="E13" s="2" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="14" spans="1:5" ht="57.6" x14ac:dyDescent="0.3">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A14" s="2" t="s">
         <v>23</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C14" s="2" t="s">
-        <v>25</v>
+        <v>217</v>
       </c>
       <c r="D14" s="2" t="s">
-        <v>63</v>
+        <v>57</v>
       </c>
       <c r="E14" s="2" t="s">
-        <v>68</v>
+        <v>214</v>
       </c>
     </row>
     <row r="15" spans="1:5" ht="43.2" x14ac:dyDescent="0.3">
@@ -1568,33 +2144,33 @@
         <v>23</v>
       </c>
       <c r="B15" s="2" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C15" s="2" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="D15" s="2" t="s">
-        <v>62</v>
+        <v>56</v>
       </c>
       <c r="E15" s="2" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="16" spans="1:5" ht="57.6" x14ac:dyDescent="0.3">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A16" s="2" t="s">
         <v>23</v>
       </c>
       <c r="B16" s="2" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C16" s="2" t="s">
-        <v>25</v>
+        <v>217</v>
       </c>
       <c r="D16" s="2" t="s">
-        <v>61</v>
+        <v>215</v>
       </c>
       <c r="E16" s="2" t="s">
-        <v>66</v>
+        <v>216</v>
       </c>
     </row>
     <row r="17" spans="1:5" ht="43.2" x14ac:dyDescent="0.3">
@@ -1602,16 +2178,16 @@
         <v>23</v>
       </c>
       <c r="B17" s="2" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C17" s="3" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="D17" s="2" t="s">
-        <v>60</v>
+        <v>55</v>
       </c>
       <c r="E17" s="2" t="s">
-        <v>65</v>
+        <v>59</v>
       </c>
     </row>
     <row r="18" spans="1:5" ht="61.2" x14ac:dyDescent="0.3">
@@ -1619,16 +2195,16 @@
         <v>23</v>
       </c>
       <c r="B18" s="2" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C18" s="2" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="D18" s="2" t="s">
-        <v>57</v>
+        <v>52</v>
       </c>
       <c r="E18" s="2" t="s">
-        <v>58</v>
+        <v>53</v>
       </c>
     </row>
     <row r="19" spans="1:5" ht="61.2" x14ac:dyDescent="0.3">
@@ -1636,16 +2212,16 @@
         <v>23</v>
       </c>
       <c r="B19" s="2" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C19" s="2" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="D19" s="2" t="s">
-        <v>56</v>
+        <v>51</v>
       </c>
       <c r="E19" s="2" t="s">
-        <v>59</v>
+        <v>54</v>
       </c>
     </row>
     <row r="20" spans="1:5" ht="75.599999999999994" x14ac:dyDescent="0.3">
@@ -1653,16 +2229,16 @@
         <v>23</v>
       </c>
       <c r="B20" s="2" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C20" s="2" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="D20" s="2" t="s">
-        <v>55</v>
+        <v>50</v>
       </c>
       <c r="E20" s="2" t="s">
-        <v>71</v>
+        <v>63</v>
       </c>
     </row>
     <row r="21" spans="1:5" ht="75.599999999999994" x14ac:dyDescent="0.3">
@@ -1670,16 +2246,16 @@
         <v>23</v>
       </c>
       <c r="B21" s="2" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C21" s="2" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="D21" s="2" t="s">
-        <v>54</v>
+        <v>49</v>
       </c>
       <c r="E21" s="2" t="s">
-        <v>72</v>
+        <v>64</v>
       </c>
     </row>
     <row r="22" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
@@ -1687,16 +2263,16 @@
         <v>23</v>
       </c>
       <c r="B22" s="2" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C22" s="2" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="D22" s="2" t="s">
-        <v>53</v>
+        <v>48</v>
       </c>
       <c r="E22" s="2" t="s">
-        <v>51</v>
+        <v>46</v>
       </c>
     </row>
     <row r="23" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
@@ -1704,16 +2280,16 @@
         <v>23</v>
       </c>
       <c r="B23" s="2" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C23" s="2" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="D23" s="2" t="s">
-        <v>50</v>
+        <v>45</v>
       </c>
       <c r="E23" s="2" t="s">
-        <v>52</v>
+        <v>47</v>
       </c>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.3">
@@ -1721,16 +2297,1019 @@
         <v>23</v>
       </c>
       <c r="B24" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="C24" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="C24" s="2" t="s">
-        <v>41</v>
-      </c>
       <c r="D24" s="2" t="s">
-        <v>48</v>
+        <v>43</v>
       </c>
       <c r="E24" s="2" t="s">
-        <v>49</v>
+        <v>44</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A26" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="B26" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="C26" s="2" t="s">
+        <v>95</v>
+      </c>
+      <c r="D26" s="2" t="s">
+        <v>97</v>
+      </c>
+      <c r="E26" s="2" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A27" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="B27" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="C27" s="2" t="s">
+        <v>95</v>
+      </c>
+      <c r="D27" s="2" t="s">
+        <v>98</v>
+      </c>
+      <c r="E27" s="2" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A28" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="B28" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="C28" s="2" t="s">
+        <v>95</v>
+      </c>
+      <c r="D28" s="2" t="s">
+        <v>99</v>
+      </c>
+      <c r="E28" s="2" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A29" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="B29" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="C29" s="2" t="s">
+        <v>95</v>
+      </c>
+      <c r="D29" s="2" t="s">
+        <v>100</v>
+      </c>
+      <c r="E29" s="2" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A30" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="B30" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="C30" s="2" t="s">
+        <v>95</v>
+      </c>
+      <c r="D30" s="2" t="s">
+        <v>101</v>
+      </c>
+      <c r="E30" s="2" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A31" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="B31" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="C31" s="2" t="s">
+        <v>95</v>
+      </c>
+      <c r="D31" s="2" t="s">
+        <v>102</v>
+      </c>
+      <c r="E31" s="2" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A32" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="B32" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="C32" s="2" t="s">
+        <v>95</v>
+      </c>
+      <c r="D32" s="2" t="s">
+        <v>103</v>
+      </c>
+      <c r="E32" s="2" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A33" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="B33" s="2" t="s">
+        <v>73</v>
+      </c>
+      <c r="C33" s="2" t="s">
+        <v>95</v>
+      </c>
+      <c r="D33" s="2" t="s">
+        <v>104</v>
+      </c>
+      <c r="E33" s="2" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="34" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A34" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="B34" s="2" t="s">
+        <v>74</v>
+      </c>
+      <c r="C34" s="2" t="s">
+        <v>95</v>
+      </c>
+      <c r="D34" s="2" t="s">
+        <v>105</v>
+      </c>
+      <c r="E34" s="2" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="35" spans="1:5" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A35" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="B35" s="2" t="s">
+        <v>75</v>
+      </c>
+      <c r="C35" s="2" t="s">
+        <v>95</v>
+      </c>
+      <c r="D35" s="2" t="s">
+        <v>106</v>
+      </c>
+      <c r="E35" s="2" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="36" spans="1:5" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A36" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="B36" s="2" t="s">
+        <v>76</v>
+      </c>
+      <c r="C36" s="2" t="s">
+        <v>95</v>
+      </c>
+      <c r="D36" s="2" t="s">
+        <v>107</v>
+      </c>
+      <c r="E36" s="2" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="37" spans="1:5" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A37" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="B37" s="2" t="s">
+        <v>77</v>
+      </c>
+      <c r="C37" s="2" t="s">
+        <v>95</v>
+      </c>
+      <c r="D37" s="2" t="s">
+        <v>108</v>
+      </c>
+      <c r="E37" s="2" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="38" spans="1:5" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A38" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="B38" s="2" t="s">
+        <v>78</v>
+      </c>
+      <c r="C38" s="2" t="s">
+        <v>95</v>
+      </c>
+      <c r="D38" s="2" t="s">
+        <v>109</v>
+      </c>
+      <c r="E38" s="2" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="39" spans="1:5" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A39" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="B39" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="C39" s="2" t="s">
+        <v>95</v>
+      </c>
+      <c r="D39" s="2" t="s">
+        <v>110</v>
+      </c>
+      <c r="E39" s="2" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="40" spans="1:5" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A40" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="B40" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="C40" s="2" t="s">
+        <v>95</v>
+      </c>
+      <c r="D40" s="2" t="s">
+        <v>111</v>
+      </c>
+      <c r="E40" s="2" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="41" spans="1:5" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A41" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="B41" s="2" t="s">
+        <v>81</v>
+      </c>
+      <c r="C41" s="2" t="s">
+        <v>95</v>
+      </c>
+      <c r="D41" s="2" t="s">
+        <v>112</v>
+      </c>
+      <c r="E41" s="2" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="42" spans="1:5" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A42" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="B42" s="2" t="s">
+        <v>82</v>
+      </c>
+      <c r="C42" s="2" t="s">
+        <v>95</v>
+      </c>
+      <c r="D42" s="2" t="s">
+        <v>113</v>
+      </c>
+      <c r="E42" s="2" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="43" spans="1:5" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A43" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="B43" s="2" t="s">
+        <v>83</v>
+      </c>
+      <c r="C43" s="2" t="s">
+        <v>95</v>
+      </c>
+      <c r="D43" s="2" t="s">
+        <v>114</v>
+      </c>
+      <c r="E43" s="2" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="44" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A44" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="B44" s="2" t="s">
+        <v>84</v>
+      </c>
+      <c r="C44" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="D44" s="2" t="s">
+        <v>115</v>
+      </c>
+      <c r="E44" s="2" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="45" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A45" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="B45" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="C45" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="D45" s="2" t="s">
+        <v>116</v>
+      </c>
+      <c r="E45" s="2" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="46" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A46" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="B46" s="2" t="s">
+        <v>86</v>
+      </c>
+      <c r="C46" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="D46" s="2" t="s">
+        <v>117</v>
+      </c>
+      <c r="E46" s="2" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="47" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A47" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="B47" s="2" t="s">
+        <v>87</v>
+      </c>
+      <c r="C47" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="D47" s="2" t="s">
+        <v>118</v>
+      </c>
+      <c r="E47" s="2" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="48" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A48" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="B48" s="2" t="s">
+        <v>88</v>
+      </c>
+      <c r="C48" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="D48" s="2" t="s">
+        <v>119</v>
+      </c>
+      <c r="E48" s="2" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="49" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A49" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="B49" s="2" t="s">
+        <v>89</v>
+      </c>
+      <c r="C49" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="D49" s="2" t="s">
+        <v>120</v>
+      </c>
+      <c r="E49" s="2" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="50" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A50" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="B50" s="2" t="s">
+        <v>90</v>
+      </c>
+      <c r="C50" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="D50" s="2" t="s">
+        <v>121</v>
+      </c>
+      <c r="E50" s="2" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="51" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A51" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="B51" s="2" t="s">
+        <v>91</v>
+      </c>
+      <c r="C51" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="D51" s="2" t="s">
+        <v>122</v>
+      </c>
+      <c r="E51" s="2" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="52" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A52" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="B52" s="2" t="s">
+        <v>92</v>
+      </c>
+      <c r="C52" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="D52" s="2" t="s">
+        <v>123</v>
+      </c>
+      <c r="E52" s="2" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="53" spans="1:5" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="A53" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="B53" s="2" t="s">
+        <v>93</v>
+      </c>
+      <c r="C53" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="D53" s="2" t="s">
+        <v>124</v>
+      </c>
+      <c r="E53" s="2" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="54" spans="1:5" ht="72" x14ac:dyDescent="0.3">
+      <c r="A54" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="B54" s="2" t="s">
+        <v>94</v>
+      </c>
+      <c r="C54" s="2" t="s">
+        <v>96</v>
+      </c>
+      <c r="D54" s="2" t="s">
+        <v>125</v>
+      </c>
+      <c r="E54" s="2" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="56" spans="1:5" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A56" s="2" t="s">
+        <v>155</v>
+      </c>
+      <c r="B56" s="2" t="s">
+        <v>156</v>
+      </c>
+      <c r="C56" s="2" t="s">
+        <v>217</v>
+      </c>
+      <c r="D56" s="2" t="s">
+        <v>218</v>
+      </c>
+      <c r="E56" s="2" t="s">
+        <v>232</v>
+      </c>
+    </row>
+    <row r="57" spans="1:5" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="A57" s="2" t="s">
+        <v>155</v>
+      </c>
+      <c r="B57" s="2" t="s">
+        <v>157</v>
+      </c>
+      <c r="C57" s="2" t="s">
+        <v>217</v>
+      </c>
+      <c r="D57" s="2" t="s">
+        <v>219</v>
+      </c>
+      <c r="E57" s="2" t="s">
+        <v>233</v>
+      </c>
+    </row>
+    <row r="58" spans="1:5" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A58" s="2" t="s">
+        <v>155</v>
+      </c>
+      <c r="B58" s="2" t="s">
+        <v>158</v>
+      </c>
+      <c r="C58" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="D58" s="2" t="s">
+        <v>220</v>
+      </c>
+      <c r="E58" s="2" t="s">
+        <v>234</v>
+      </c>
+    </row>
+    <row r="59" spans="1:5" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A59" s="2" t="s">
+        <v>155</v>
+      </c>
+      <c r="B59" s="2" t="s">
+        <v>159</v>
+      </c>
+      <c r="C59" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="D59" s="2" t="s">
+        <v>221</v>
+      </c>
+      <c r="E59" s="2" t="s">
+        <v>235</v>
+      </c>
+    </row>
+    <row r="60" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A60" s="2" t="s">
+        <v>155</v>
+      </c>
+      <c r="B60" s="2" t="s">
+        <v>160</v>
+      </c>
+      <c r="C60" s="2" t="s">
+        <v>187</v>
+      </c>
+      <c r="D60" s="2" t="s">
+        <v>222</v>
+      </c>
+      <c r="E60" s="2" t="s">
+        <v>236</v>
+      </c>
+    </row>
+    <row r="61" spans="1:5" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="A61" s="2" t="s">
+        <v>155</v>
+      </c>
+      <c r="B61" s="2" t="s">
+        <v>161</v>
+      </c>
+      <c r="C61" s="2" t="s">
+        <v>217</v>
+      </c>
+      <c r="D61" s="2" t="s">
+        <v>223</v>
+      </c>
+      <c r="E61" s="2" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="62" spans="1:5" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="A62" s="2" t="s">
+        <v>155</v>
+      </c>
+      <c r="B62" s="2" t="s">
+        <v>162</v>
+      </c>
+      <c r="C62" s="2" t="s">
+        <v>217</v>
+      </c>
+      <c r="D62" s="2" t="s">
+        <v>224</v>
+      </c>
+      <c r="E62" s="2" t="s">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="63" spans="1:5" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A63" s="2" t="s">
+        <v>155</v>
+      </c>
+      <c r="B63" s="2" t="s">
+        <v>163</v>
+      </c>
+      <c r="C63" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="D63" s="2" t="s">
+        <v>225</v>
+      </c>
+      <c r="E63" s="2" t="s">
+        <v>239</v>
+      </c>
+    </row>
+    <row r="64" spans="1:5" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A64" s="2" t="s">
+        <v>155</v>
+      </c>
+      <c r="B64" s="2" t="s">
+        <v>164</v>
+      </c>
+      <c r="C64" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="D64" s="2" t="s">
+        <v>226</v>
+      </c>
+      <c r="E64" s="2" t="s">
+        <v>241</v>
+      </c>
+    </row>
+    <row r="65" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A65" s="2" t="s">
+        <v>155</v>
+      </c>
+      <c r="B65" s="2" t="s">
+        <v>169</v>
+      </c>
+      <c r="C65" s="2" t="s">
+        <v>217</v>
+      </c>
+      <c r="D65" s="2" t="s">
+        <v>227</v>
+      </c>
+      <c r="E65" s="2" t="s">
+        <v>242</v>
+      </c>
+    </row>
+    <row r="66" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A66" s="2" t="s">
+        <v>155</v>
+      </c>
+      <c r="B66" s="2" t="s">
+        <v>165</v>
+      </c>
+      <c r="C66" s="2" t="s">
+        <v>188</v>
+      </c>
+      <c r="D66" s="2" t="s">
+        <v>228</v>
+      </c>
+      <c r="E66" s="2" t="s">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="67" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A67" s="2" t="s">
+        <v>155</v>
+      </c>
+      <c r="B67" s="2" t="s">
+        <v>166</v>
+      </c>
+      <c r="C67" s="2" t="s">
+        <v>217</v>
+      </c>
+      <c r="D67" s="2" t="s">
+        <v>230</v>
+      </c>
+      <c r="E67" s="2" t="s">
+        <v>245</v>
+      </c>
+    </row>
+    <row r="68" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A68" s="2" t="s">
+        <v>155</v>
+      </c>
+      <c r="B68" s="2" t="s">
+        <v>167</v>
+      </c>
+      <c r="C68" s="2" t="s">
+        <v>188</v>
+      </c>
+      <c r="D68" s="2" t="s">
+        <v>229</v>
+      </c>
+      <c r="E68" s="2" t="s">
+        <v>244</v>
+      </c>
+    </row>
+    <row r="69" spans="1:5" ht="144" x14ac:dyDescent="0.3">
+      <c r="A69" s="2" t="s">
+        <v>155</v>
+      </c>
+      <c r="B69" s="2" t="s">
+        <v>168</v>
+      </c>
+      <c r="C69" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="D69" s="2" t="s">
+        <v>231</v>
+      </c>
+      <c r="E69" s="2" t="s">
+        <v>246</v>
+      </c>
+    </row>
+    <row r="71" spans="1:5" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A71" s="2" t="s">
+        <v>186</v>
+      </c>
+      <c r="B71" s="2" t="s">
+        <v>170</v>
+      </c>
+      <c r="C71" s="2" t="s">
+        <v>192</v>
+      </c>
+      <c r="D71" s="2" t="s">
+        <v>193</v>
+      </c>
+      <c r="E71" s="2" t="s">
+        <v>247</v>
+      </c>
+    </row>
+    <row r="72" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A72" s="2" t="s">
+        <v>186</v>
+      </c>
+      <c r="B72" s="2" t="s">
+        <v>171</v>
+      </c>
+      <c r="C72" s="2" t="s">
+        <v>194</v>
+      </c>
+      <c r="D72" s="2" t="s">
+        <v>195</v>
+      </c>
+      <c r="E72" s="2" t="s">
+        <v>248</v>
+      </c>
+    </row>
+    <row r="73" spans="1:5" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A73" s="2" t="s">
+        <v>186</v>
+      </c>
+      <c r="B73" s="2" t="s">
+        <v>172</v>
+      </c>
+      <c r="C73" s="2" t="s">
+        <v>95</v>
+      </c>
+      <c r="D73" s="2" t="s">
+        <v>196</v>
+      </c>
+      <c r="E73" s="2" t="s">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="74" spans="1:5" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="A74" s="2" t="s">
+        <v>186</v>
+      </c>
+      <c r="B74" s="2" t="s">
+        <v>173</v>
+      </c>
+      <c r="C74" s="2" t="s">
+        <v>189</v>
+      </c>
+      <c r="D74" s="2" t="s">
+        <v>197</v>
+      </c>
+      <c r="E74" s="2" t="s">
+        <v>249</v>
+      </c>
+    </row>
+    <row r="75" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A75" s="2" t="s">
+        <v>186</v>
+      </c>
+      <c r="B75" s="2" t="s">
+        <v>174</v>
+      </c>
+      <c r="C75" s="2" t="s">
+        <v>190</v>
+      </c>
+      <c r="D75" s="2" t="s">
+        <v>198</v>
+      </c>
+      <c r="E75" s="2" t="s">
+        <v>251</v>
+      </c>
+    </row>
+    <row r="76" spans="1:5" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="A76" s="2" t="s">
+        <v>186</v>
+      </c>
+      <c r="B76" s="2" t="s">
+        <v>175</v>
+      </c>
+      <c r="C76" s="2" t="s">
+        <v>95</v>
+      </c>
+      <c r="D76" s="2" t="s">
+        <v>199</v>
+      </c>
+      <c r="E76" s="2" t="s">
+        <v>252</v>
+      </c>
+    </row>
+    <row r="77" spans="1:5" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A77" s="2" t="s">
+        <v>186</v>
+      </c>
+      <c r="B77" s="2" t="s">
+        <v>176</v>
+      </c>
+      <c r="C77" s="2" t="s">
+        <v>95</v>
+      </c>
+      <c r="D77" s="2" t="s">
+        <v>200</v>
+      </c>
+      <c r="E77" s="2" t="s">
+        <v>253</v>
+      </c>
+    </row>
+    <row r="78" spans="1:5" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A78" s="2" t="s">
+        <v>186</v>
+      </c>
+      <c r="B78" s="2" t="s">
+        <v>177</v>
+      </c>
+      <c r="C78" s="2" t="s">
+        <v>95</v>
+      </c>
+      <c r="D78" s="2" t="s">
+        <v>201</v>
+      </c>
+      <c r="E78" s="2" t="s">
+        <v>254</v>
+      </c>
+    </row>
+    <row r="79" spans="1:5" ht="72" x14ac:dyDescent="0.3">
+      <c r="A79" s="2" t="s">
+        <v>186</v>
+      </c>
+      <c r="B79" s="2" t="s">
+        <v>178</v>
+      </c>
+      <c r="C79" s="2" t="s">
+        <v>95</v>
+      </c>
+      <c r="D79" s="2" t="s">
+        <v>202</v>
+      </c>
+      <c r="E79" s="2" t="s">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="80" spans="1:5" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="A80" s="2" t="s">
+        <v>186</v>
+      </c>
+      <c r="B80" s="2" t="s">
+        <v>179</v>
+      </c>
+      <c r="C80" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="D80" s="2" t="s">
+        <v>203</v>
+      </c>
+      <c r="E80" s="2" t="s">
+        <v>240</v>
+      </c>
+    </row>
+    <row r="81" spans="1:5" ht="72" x14ac:dyDescent="0.3">
+      <c r="A81" s="2" t="s">
+        <v>186</v>
+      </c>
+      <c r="B81" s="2" t="s">
+        <v>180</v>
+      </c>
+      <c r="C81" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="D81" s="2" t="s">
+        <v>204</v>
+      </c>
+      <c r="E81" s="2" t="s">
+        <v>256</v>
+      </c>
+    </row>
+    <row r="82" spans="1:5" ht="72" x14ac:dyDescent="0.3">
+      <c r="A82" s="2" t="s">
+        <v>186</v>
+      </c>
+      <c r="B82" s="2" t="s">
+        <v>181</v>
+      </c>
+      <c r="C82" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="D82" s="2" t="s">
+        <v>205</v>
+      </c>
+      <c r="E82" s="2" t="s">
+        <v>257</v>
+      </c>
+    </row>
+    <row r="83" spans="1:5" ht="129.6" x14ac:dyDescent="0.3">
+      <c r="A83" s="2" t="s">
+        <v>186</v>
+      </c>
+      <c r="B83" s="2" t="s">
+        <v>182</v>
+      </c>
+      <c r="C83" s="2" t="s">
+        <v>187</v>
+      </c>
+      <c r="D83" s="2" t="s">
+        <v>206</v>
+      </c>
+      <c r="E83" s="2" t="s">
+        <v>258</v>
+      </c>
+    </row>
+    <row r="84" spans="1:5" ht="144" x14ac:dyDescent="0.3">
+      <c r="A84" s="2" t="s">
+        <v>186</v>
+      </c>
+      <c r="B84" s="2" t="s">
+        <v>183</v>
+      </c>
+      <c r="C84" s="2" t="s">
+        <v>187</v>
+      </c>
+      <c r="D84" s="2" t="s">
+        <v>207</v>
+      </c>
+      <c r="E84" s="2" t="s">
+        <v>259</v>
+      </c>
+    </row>
+    <row r="85" spans="1:5" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A85" s="2" t="s">
+        <v>186</v>
+      </c>
+      <c r="B85" s="2" t="s">
+        <v>184</v>
+      </c>
+      <c r="C85" s="2" t="s">
+        <v>191</v>
+      </c>
+      <c r="D85" s="2" t="s">
+        <v>208</v>
+      </c>
+      <c r="E85" s="2" t="s">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="86" spans="1:5" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A86" s="2" t="s">
+        <v>186</v>
+      </c>
+      <c r="B86" s="2" t="s">
+        <v>185</v>
+      </c>
+      <c r="C86" s="2" t="s">
+        <v>191</v>
+      </c>
+      <c r="D86" s="2" t="s">
+        <v>209</v>
+      </c>
+      <c r="E86" s="2" t="s">
+        <v>260</v>
       </c>
     </row>
   </sheetData>

</xml_diff>